<commit_message>
vault backup: 2024-04-10 13:10:15
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
+++ b/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/quote-process-optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{A5D92240-C2E0-44E4-8715-FBBA2B0F3533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{473AF777-26D1-43A9-91F6-3B5350F34D80}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{A5D92240-C2E0-44E4-8715-FBBA2B0F3533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BDD3A52-CADB-476B-B486-75279B1B534E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1965" yWindow="4650" windowWidth="23235" windowHeight="1530" activeTab="2" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
+    <workbookView minimized="1" xWindow="28830" yWindow="870" windowWidth="28740" windowHeight="15420" activeTab="2" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Field Descriptions" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Edit Team" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="158">
   <si>
     <t>Add Profile</t>
   </si>
@@ -511,6 +512,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
 </sst>
 </file>
@@ -634,7 +638,43 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -649,20 +689,6 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -705,10 +731,6 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -720,16 +742,22 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -744,19 +772,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:B7" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6BE075E6-89FE-4758-9225-DA2C18ED1BE2}" name="Field" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{6958885B-EEE8-46BD-8538-5380EC30F9FC}" name="Description" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{6BE075E6-89FE-4758-9225-DA2C18ED1BE2}" name="Field" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{6958885B-EEE8-46BD-8538-5380EC30F9FC}" name="Description" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}" name="Table3" displayName="Table3" ref="A1:E16" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}" name="Table3" displayName="Table3" ref="A1:E16" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:E16" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2705EF5E-7673-46B7-8510-3E355CF13A75}" name="Team Name"/>
@@ -770,26 +802,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}" name="Table4" displayName="Table4" ref="A1:F116" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F116" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}" name="Table4" displayName="Table4" ref="A1:H116" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:H116" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="2"/>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5AA60B3A-5C22-4EF1-AC63-FFA2B35F0AB0}" name="Quote Template Name"/>
-    <tableColumn id="2" xr3:uid="{AB7FACE1-48AE-4A13-BBC5-CCCF638FE478}" name="Number" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E87ED63C-BC54-49FC-89C8-83EB2458BED5}" name="Total" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A5F807BA-08F9-41A4-9CBF-90139FB2D23D}" name="Recurring" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{620AA166-6A38-4FFB-9E56-F773F40A0C00}" name="Status" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{D73D302D-1A85-48F4-98FA-FBF948C010DD}" name="Notes"/>
+    <tableColumn id="2" xr3:uid="{AB7FACE1-48AE-4A13-BBC5-CCCF638FE478}" name="Number" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E87ED63C-BC54-49FC-89C8-83EB2458BED5}" name="Total" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A5F807BA-08F9-41A4-9CBF-90139FB2D23D}" name="Recurring" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{620AA166-6A38-4FFB-9E56-F773F40A0C00}" name="Status" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{D73D302D-1A85-48F4-98FA-FBF948C010DD}" name="Description"/>
+    <tableColumn id="7" xr3:uid="{FC6A876C-C9E6-4C0E-9FD5-68D58EECBB8E}" name="Action"/>
+    <tableColumn id="8" xr3:uid="{D12601E4-780E-4EE5-BC38-8971219B29FA}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CCC9A8D-F711-4E57-B1C3-589FC084751F}" name="Table13" displayName="Table13" ref="A1:B5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CCC9A8D-F711-4E57-B1C3-589FC084751F}" name="Table13" displayName="Table13" ref="A1:B5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:B5" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E54FF52E-4A15-4487-9838-6510910D6C97}" name="Field" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{95A31568-5DA9-4E0E-AECC-CD03CCF21147}" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{E54FF52E-4A15-4487-9838-6510910D6C97}" name="Field" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{95A31568-5DA9-4E0E-AECC-CD03CCF21147}" name="Description" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1118,7 +1156,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>
@@ -1451,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF9CB69-39A5-427C-AC5B-F48FDEB163BE}">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,9 +1503,11 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1484,10 +1524,16 @@
         <v>40</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1504,7 +1550,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1521,24 +1567,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="12">
         <v>84520</v>
       </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1555,7 +1604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1572,7 +1621,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1589,7 +1638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>48</v>
       </c>
@@ -1608,25 +1657,30 @@
       <c r="F8" s="11" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="12">
         <v>84521</v>
       </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
@@ -1643,8 +1697,10 @@
         <v>42</v>
       </c>
       <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1661,7 +1717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1678,7 +1734,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1695,7 +1751,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1712,7 +1768,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1729,7 +1785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1746,7 +1802,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1763,24 +1819,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="12">
         <v>5250</v>
       </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1797,7 +1856,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -1814,7 +1873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1831,7 +1890,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1848,7 +1907,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1865,7 +1924,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -1882,7 +1941,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1899,7 +1958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1916,7 +1975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1933,7 +1992,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1950,7 +2009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1967,7 +2026,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1984,7 +2043,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -2001,7 +2060,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2018,7 +2077,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2035,7 +2094,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>74</v>
       </c>
@@ -2052,8 +2111,10 @@
         <v>42</v>
       </c>
       <c r="F34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>75</v>
       </c>
@@ -2070,8 +2131,10 @@
         <v>42</v>
       </c>
       <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2088,7 +2151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>77</v>
       </c>
@@ -2105,8 +2168,10 @@
         <v>42</v>
       </c>
       <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>78</v>
       </c>
@@ -2123,8 +2188,10 @@
         <v>42</v>
       </c>
       <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
@@ -2141,8 +2208,10 @@
         <v>42</v>
       </c>
       <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>80</v>
       </c>
@@ -2159,8 +2228,10 @@
         <v>42</v>
       </c>
       <c r="F40" s="11"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>81</v>
       </c>
@@ -2177,8 +2248,10 @@
         <v>42</v>
       </c>
       <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>82</v>
       </c>
@@ -2195,8 +2268,10 @@
         <v>42</v>
       </c>
       <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>83</v>
       </c>
@@ -2213,8 +2288,10 @@
         <v>42</v>
       </c>
       <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2231,7 +2308,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2248,7 +2325,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>86</v>
       </c>
@@ -2265,8 +2342,10 @@
         <v>42</v>
       </c>
       <c r="F46" s="11"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>87</v>
       </c>
@@ -2283,8 +2362,10 @@
         <v>42</v>
       </c>
       <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>88</v>
       </c>
@@ -2301,8 +2382,10 @@
         <v>42</v>
       </c>
       <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -2319,7 +2402,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>90</v>
       </c>
@@ -2336,8 +2419,10 @@
         <v>42</v>
       </c>
       <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -2354,7 +2439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2371,7 +2456,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -2388,7 +2473,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2405,7 +2490,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>95</v>
       </c>
@@ -2422,7 +2507,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -2439,7 +2524,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>97</v>
       </c>
@@ -2456,7 +2541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2473,7 +2558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -2490,7 +2575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -2507,7 +2592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2524,7 +2609,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -2541,7 +2626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -2558,7 +2643,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>104</v>
       </c>
@@ -2575,7 +2660,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>105</v>
       </c>
@@ -2592,7 +2677,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>106</v>
       </c>
@@ -2609,7 +2694,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>107</v>
       </c>
@@ -2626,7 +2711,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>108</v>
       </c>
@@ -2643,7 +2728,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>109</v>
       </c>
@@ -2660,7 +2745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>109</v>
       </c>
@@ -2677,7 +2762,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>110</v>
       </c>
@@ -2694,7 +2779,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>111</v>
       </c>
@@ -2711,7 +2796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>112</v>
       </c>
@@ -2728,7 +2813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>113</v>
       </c>
@@ -2745,7 +2830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>114</v>
       </c>
@@ -2762,7 +2847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>115</v>
       </c>
@@ -2779,7 +2864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>116</v>
       </c>
@@ -2796,8 +2881,10 @@
         <v>42</v>
       </c>
       <c r="F77" s="11"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+    </row>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>117</v>
       </c>
@@ -2814,7 +2901,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>118</v>
       </c>
@@ -2831,7 +2918,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>119</v>
       </c>
@@ -2848,7 +2935,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>120</v>
       </c>
@@ -2865,7 +2952,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>121</v>
       </c>
@@ -2882,8 +2969,10 @@
         <v>42</v>
       </c>
       <c r="F82" s="11"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>122</v>
       </c>
@@ -2900,8 +2989,10 @@
         <v>42</v>
       </c>
       <c r="F83" s="11"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+    </row>
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>123</v>
       </c>
@@ -2918,7 +3009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>124</v>
       </c>
@@ -2935,8 +3026,10 @@
         <v>42</v>
       </c>
       <c r="F85" s="11"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>125</v>
       </c>
@@ -2953,8 +3046,10 @@
         <v>42</v>
       </c>
       <c r="F86" s="11"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>126</v>
       </c>
@@ -2971,7 +3066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>126</v>
       </c>
@@ -2988,7 +3083,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>126</v>
       </c>
@@ -3005,7 +3100,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>127</v>
       </c>
@@ -3022,7 +3117,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>128</v>
       </c>
@@ -3039,7 +3134,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>129</v>
       </c>
@@ -3056,8 +3151,10 @@
         <v>42</v>
       </c>
       <c r="F92" s="11"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+    </row>
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>130</v>
       </c>
@@ -3074,7 +3171,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>131</v>
       </c>
@@ -3091,8 +3188,10 @@
         <v>42</v>
       </c>
       <c r="F94" s="11"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+    </row>
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>132</v>
       </c>
@@ -3109,7 +3208,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>133</v>
       </c>
@@ -3126,8 +3225,10 @@
         <v>42</v>
       </c>
       <c r="F96" s="11"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+    </row>
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>134</v>
       </c>
@@ -3144,7 +3245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>135</v>
       </c>
@@ -3161,7 +3262,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>136</v>
       </c>
@@ -3178,7 +3279,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>137</v>
       </c>
@@ -3195,8 +3296,10 @@
         <v>42</v>
       </c>
       <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+    </row>
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>138</v>
       </c>
@@ -3213,7 +3316,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>139</v>
       </c>
@@ -3230,8 +3333,10 @@
         <v>42</v>
       </c>
       <c r="F102" s="11"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="11"/>
+      <c r="H102" s="11"/>
+    </row>
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>140</v>
       </c>
@@ -3248,7 +3353,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>141</v>
       </c>
@@ -3265,7 +3370,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>142</v>
       </c>
@@ -3282,7 +3387,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>143</v>
       </c>
@@ -3299,7 +3404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>144</v>
       </c>
@@ -3316,7 +3421,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>145</v>
       </c>
@@ -3333,7 +3438,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>146</v>
       </c>
@@ -3350,7 +3455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>147</v>
       </c>
@@ -3367,7 +3472,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>148</v>
       </c>
@@ -3384,7 +3489,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -3401,7 +3506,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>150</v>
       </c>
@@ -3418,8 +3523,10 @@
         <v>42</v>
       </c>
       <c r="F113" s="11"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>151</v>
       </c>
@@ -3436,8 +3543,10 @@
         <v>42</v>
       </c>
       <c r="F114" s="11"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>152</v>
       </c>
@@ -3454,8 +3563,10 @@
         <v>42</v>
       </c>
       <c r="F115" s="11"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
+    </row>
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>153</v>
       </c>
@@ -3473,6 +3584,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G116" xr:uid="{200E3D86-4210-41AF-B914-810C92509338}">
+      <formula1>"Deprecate, Modify, Consolidate, N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3488,7 +3604,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
vault backup: 2024-04-11 09:28:33
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
+++ b/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="123" documentId="8_{A5D92240-C2E0-44E4-8715-FBBA2B0F3533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BDD3A52-CADB-476B-B486-75279B1B534E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="28830" yWindow="870" windowWidth="28740" windowHeight="15420" activeTab="2" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
+    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Field Descriptions" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Edit Team" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -638,31 +637,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -703,6 +678,14 @@
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -772,23 +755,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:B7" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6BE075E6-89FE-4758-9225-DA2C18ED1BE2}" name="Field" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6958885B-EEE8-46BD-8538-5380EC30F9FC}" name="Description" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{6BE075E6-89FE-4758-9225-DA2C18ED1BE2}" name="Field" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6958885B-EEE8-46BD-8538-5380EC30F9FC}" name="Description" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}" name="Table3" displayName="Table3" ref="A1:E16" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}" name="Table3" displayName="Table3" ref="A1:E16" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:E16" xr:uid="{375F0321-FC23-446E-A31A-0A092C64B0BF}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2705EF5E-7673-46B7-8510-3E355CF13A75}" name="Team Name"/>
@@ -802,18 +781,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}" name="Table4" displayName="Table4" ref="A1:H116" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}" name="Table4" displayName="Table4" ref="A1:H116" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:H116" xr:uid="{A752994E-AC3D-42A6-83AF-EB2559080BDF}">
     <filterColumn colId="0">
-      <colorFilter dxfId="2"/>
+      <colorFilter dxfId="8"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5AA60B3A-5C22-4EF1-AC63-FFA2B35F0AB0}" name="Quote Template Name"/>
-    <tableColumn id="2" xr3:uid="{AB7FACE1-48AE-4A13-BBC5-CCCF638FE478}" name="Number" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E87ED63C-BC54-49FC-89C8-83EB2458BED5}" name="Total" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{A5F807BA-08F9-41A4-9CBF-90139FB2D23D}" name="Recurring" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{620AA166-6A38-4FFB-9E56-F773F40A0C00}" name="Status" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AB7FACE1-48AE-4A13-BBC5-CCCF638FE478}" name="Number" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{E87ED63C-BC54-49FC-89C8-83EB2458BED5}" name="Total" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A5F807BA-08F9-41A4-9CBF-90139FB2D23D}" name="Recurring" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{620AA166-6A38-4FFB-9E56-F773F40A0C00}" name="Status" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{D73D302D-1A85-48F4-98FA-FBF948C010DD}" name="Description"/>
     <tableColumn id="7" xr3:uid="{FC6A876C-C9E6-4C0E-9FD5-68D58EECBB8E}" name="Action"/>
     <tableColumn id="8" xr3:uid="{D12601E4-780E-4EE5-BC38-8971219B29FA}" name="Notes"/>
@@ -823,11 +802,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CCC9A8D-F711-4E57-B1C3-589FC084751F}" name="Table13" displayName="Table13" ref="A1:B5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CCC9A8D-F711-4E57-B1C3-589FC084751F}" name="Table13" displayName="Table13" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B5" xr:uid="{BA5122E7-5189-4468-BF8F-0683950E4BA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E54FF52E-4A15-4487-9838-6510910D6C97}" name="Field" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{95A31568-5DA9-4E0E-AECC-CD03CCF21147}" name="Description" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{E54FF52E-4A15-4487-9838-6510910D6C97}" name="Field" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{95A31568-5DA9-4E0E-AECC-CD03CCF21147}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1492,7 +1471,7 @@
   <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
vault backup: 2024-04-19 08:56:49
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
+++ b/projects/quote-process-optimization/cwsell-teams-matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/quote-process-optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{A5D92240-C2E0-44E4-8715-FBBA2B0F3533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81D9917C-C7E3-4DE9-987A-199FAB555797}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{A5D92240-C2E0-44E4-8715-FBBA2B0F3533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17972CE4-B04A-41B9-8E58-41D43E6BA59E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6107A567-3E09-47F5-8C1B-BDEC155DBC75}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Field Descriptions" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,13 +535,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -561,17 +554,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -588,12 +576,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,31 +597,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -1198,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC182DA-AFA1-48C9-B759-1603FF1DFEC8}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,19 +1417,19 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="14" t="b">
+      <c r="C16" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="14" t="b">
+      <c r="D16" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1458,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF9CB69-39A5-427C-AC5B-F48FDEB163BE}">
   <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>